<commit_message>
Added Filters to all columns
Filters in each column added for drop-down list of all possible values; helpful for:
-data inspection
-invalid values removal
-filtering
</commit_message>
<xml_diff>
--- a/Excel Project Dataset.xlsx
+++ b/Excel Project Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanbolin/Desktop/Excel-Tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10899DA0-EDD2-BE4E-85FE-B5B47788A815}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E209BE8-E30A-7F40-B737-AF24DA56E39E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="640" windowWidth="15120" windowHeight="19000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bike_buyers" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">bike_buyers!$A$1:$M$1001</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Working Sheet'!$A$1:$M$1001</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -43133,7 +43134,7 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -84184,6 +84185,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:M1001" xr:uid="{66FD7F5C-B0E9-2C42-9475-D5B2E56CEB99}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Added Histogram for Bike Purchase by Income and Gender
</commit_message>
<xml_diff>
--- a/Excel Project Dataset.xlsx
+++ b/Excel Project Dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanbolin/Desktop/Excel-Tutorial/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEAB0521-5B91-FB41-BC84-D40567C42384}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE157545-CD26-C64F-B654-92C07892DB1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15120" yWindow="640" windowWidth="15420" windowHeight="19000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15120" yWindow="640" windowWidth="16640" windowHeight="19000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bike_buyers" sheetId="1" r:id="rId1"/>
@@ -740,6 +740,1076 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[Excel Project Dataset.xlsx]Pivot Table!PivotTable1</c:name>
+    <c:fmtId val="1"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.22124759405074368"/>
+          <c:y val="7.407407407407407E-2"/>
+          <c:w val="0.76549803149606299"/>
+          <c:h val="0.8416746864975212"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$B$3:$B$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>No</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pivot Table'!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Female</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Male</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$B$5:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>53440</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>56208.178438661707</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-87D5-3144-908C-283D83F7094F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Pivot Table'!$C$3:$C$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Yes</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Pivot Table'!$A$5:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Female</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Male</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Pivot Table'!$C$5:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>55774.058577405856</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60123.966942148763</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-87D5-3144-908C-283D83F7094F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1087779920"/>
+        <c:axId val="1252678272"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1087779920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1252678272"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1252678272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1087779920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE9A0342-0308-F847-C827-51145D03BA50}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16811,7 +17881,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1A85D23C-6514-4F47-83FD-296CCF453A40}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1A85D23C-6514-4F47-83FD-296CCF453A40}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="3">
   <location ref="A3:D7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="14">
     <pivotField showAll="0"/>
@@ -16872,6 +17942,56 @@
   <dataFields count="1">
     <dataField name="Average of Income" fld="3" subtotal="average" baseField="0" baseItem="0"/>
   </dataFields>
+  <chartFormats count="4">
+    <chartFormat chart="0" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="0" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="1" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="13" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -104375,8 +105495,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DDBA69B-5B2F-B949-B318-727D54BF42DC}">
   <dimension ref="A3:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -104452,6 +105572,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>